<commit_message>
view and logic updated
</commit_message>
<xml_diff>
--- a/test dataset.xlsx
+++ b/test dataset.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F41461-D1D4-4BB4-B232-8D3D99DE181F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48639F44-687A-4EF8-9C35-0D4DA3395516}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="21">
   <si>
     <t>p</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>v</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> d</t>
   </si>
 </sst>
 </file>
@@ -394,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W16"/>
+  <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:W16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:W32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -407,37 +413,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="M1" t="s">
         <v>2</v>
@@ -1535,6 +1523,1124 @@
         <v>12</v>
       </c>
       <c r="W16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" t="s">
+        <v>2</v>
+      </c>
+      <c r="N17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O17" t="s">
+        <v>9</v>
+      </c>
+      <c r="P17" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" t="s">
+        <v>9</v>
+      </c>
+      <c r="S17" t="s">
+        <v>10</v>
+      </c>
+      <c r="T17" t="s">
+        <v>0</v>
+      </c>
+      <c r="U17" t="s">
+        <v>7</v>
+      </c>
+      <c r="V17" t="s">
+        <v>2</v>
+      </c>
+      <c r="W17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" t="s">
+        <v>7</v>
+      </c>
+      <c r="K18" t="s">
+        <v>8</v>
+      </c>
+      <c r="L18" t="s">
+        <v>6</v>
+      </c>
+      <c r="M18" t="s">
+        <v>2</v>
+      </c>
+      <c r="N18" t="s">
+        <v>2</v>
+      </c>
+      <c r="O18" t="s">
+        <v>9</v>
+      </c>
+      <c r="P18" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>0</v>
+      </c>
+      <c r="R18" t="s">
+        <v>9</v>
+      </c>
+      <c r="S18" t="s">
+        <v>10</v>
+      </c>
+      <c r="T18" t="s">
+        <v>0</v>
+      </c>
+      <c r="U18" t="s">
+        <v>3</v>
+      </c>
+      <c r="V18" t="s">
+        <v>3</v>
+      </c>
+      <c r="W18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K19" t="s">
+        <v>8</v>
+      </c>
+      <c r="L19" t="s">
+        <v>6</v>
+      </c>
+      <c r="M19" t="s">
+        <v>2</v>
+      </c>
+      <c r="N19" t="s">
+        <v>2</v>
+      </c>
+      <c r="O19" t="s">
+        <v>9</v>
+      </c>
+      <c r="P19" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>0</v>
+      </c>
+      <c r="R19" t="s">
+        <v>9</v>
+      </c>
+      <c r="S19" t="s">
+        <v>10</v>
+      </c>
+      <c r="T19" t="s">
+        <v>0</v>
+      </c>
+      <c r="U19" t="s">
+        <v>3</v>
+      </c>
+      <c r="V19" t="s">
+        <v>3</v>
+      </c>
+      <c r="W19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" t="s">
+        <v>3</v>
+      </c>
+      <c r="J20" t="s">
+        <v>3</v>
+      </c>
+      <c r="K20" t="s">
+        <v>8</v>
+      </c>
+      <c r="L20" t="s">
+        <v>8</v>
+      </c>
+      <c r="M20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O20" t="s">
+        <v>9</v>
+      </c>
+      <c r="P20" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>0</v>
+      </c>
+      <c r="R20" t="s">
+        <v>9</v>
+      </c>
+      <c r="S20" t="s">
+        <v>10</v>
+      </c>
+      <c r="T20" t="s">
+        <v>0</v>
+      </c>
+      <c r="U20" t="s">
+        <v>7</v>
+      </c>
+      <c r="V20" t="s">
+        <v>2</v>
+      </c>
+      <c r="W20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" t="s">
+        <v>7</v>
+      </c>
+      <c r="K21" t="s">
+        <v>4</v>
+      </c>
+      <c r="L21" t="s">
+        <v>8</v>
+      </c>
+      <c r="M21" t="s">
+        <v>2</v>
+      </c>
+      <c r="N21" t="s">
+        <v>2</v>
+      </c>
+      <c r="O21" t="s">
+        <v>9</v>
+      </c>
+      <c r="P21" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>0</v>
+      </c>
+      <c r="R21" t="s">
+        <v>9</v>
+      </c>
+      <c r="S21" t="s">
+        <v>10</v>
+      </c>
+      <c r="T21" t="s">
+        <v>8</v>
+      </c>
+      <c r="U21" t="s">
+        <v>3</v>
+      </c>
+      <c r="V21" t="s">
+        <v>13</v>
+      </c>
+      <c r="W21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22" t="s">
+        <v>8</v>
+      </c>
+      <c r="L22" t="s">
+        <v>6</v>
+      </c>
+      <c r="M22" t="s">
+        <v>2</v>
+      </c>
+      <c r="N22" t="s">
+        <v>2</v>
+      </c>
+      <c r="O22" t="s">
+        <v>9</v>
+      </c>
+      <c r="P22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>0</v>
+      </c>
+      <c r="R22" t="s">
+        <v>9</v>
+      </c>
+      <c r="S22" t="s">
+        <v>10</v>
+      </c>
+      <c r="T22" t="s">
+        <v>0</v>
+      </c>
+      <c r="U22" t="s">
+        <v>7</v>
+      </c>
+      <c r="V22" t="s">
+        <v>3</v>
+      </c>
+      <c r="W22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" t="s">
+        <v>8</v>
+      </c>
+      <c r="L23" t="s">
+        <v>6</v>
+      </c>
+      <c r="M23" t="s">
+        <v>2</v>
+      </c>
+      <c r="N23" t="s">
+        <v>2</v>
+      </c>
+      <c r="O23" t="s">
+        <v>9</v>
+      </c>
+      <c r="P23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>0</v>
+      </c>
+      <c r="R23" t="s">
+        <v>9</v>
+      </c>
+      <c r="S23" t="s">
+        <v>10</v>
+      </c>
+      <c r="T23" t="s">
+        <v>0</v>
+      </c>
+      <c r="U23" t="s">
+        <v>7</v>
+      </c>
+      <c r="V23" t="s">
+        <v>3</v>
+      </c>
+      <c r="W23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" t="s">
+        <v>3</v>
+      </c>
+      <c r="K24" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24" t="s">
+        <v>6</v>
+      </c>
+      <c r="M24" t="s">
+        <v>2</v>
+      </c>
+      <c r="N24" t="s">
+        <v>2</v>
+      </c>
+      <c r="O24" t="s">
+        <v>9</v>
+      </c>
+      <c r="P24" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>0</v>
+      </c>
+      <c r="R24" t="s">
+        <v>9</v>
+      </c>
+      <c r="S24" t="s">
+        <v>10</v>
+      </c>
+      <c r="T24" t="s">
+        <v>0</v>
+      </c>
+      <c r="U24" t="s">
+        <v>3</v>
+      </c>
+      <c r="V24" t="s">
+        <v>2</v>
+      </c>
+      <c r="W24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" t="s">
+        <v>3</v>
+      </c>
+      <c r="J25" t="s">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
+        <v>8</v>
+      </c>
+      <c r="L25" t="s">
+        <v>8</v>
+      </c>
+      <c r="M25" t="s">
+        <v>2</v>
+      </c>
+      <c r="N25" t="s">
+        <v>2</v>
+      </c>
+      <c r="O25" t="s">
+        <v>9</v>
+      </c>
+      <c r="P25" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>0</v>
+      </c>
+      <c r="R25" t="s">
+        <v>9</v>
+      </c>
+      <c r="S25" t="s">
+        <v>10</v>
+      </c>
+      <c r="T25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U25" t="s">
+        <v>7</v>
+      </c>
+      <c r="V25" t="s">
+        <v>18</v>
+      </c>
+      <c r="W25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26" t="s">
+        <v>8</v>
+      </c>
+      <c r="L26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M26" t="s">
+        <v>2</v>
+      </c>
+      <c r="N26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O26" t="s">
+        <v>9</v>
+      </c>
+      <c r="P26" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>0</v>
+      </c>
+      <c r="R26" t="s">
+        <v>9</v>
+      </c>
+      <c r="S26" t="s">
+        <v>10</v>
+      </c>
+      <c r="T26" t="s">
+        <v>0</v>
+      </c>
+      <c r="U26" t="s">
+        <v>7</v>
+      </c>
+      <c r="V26" t="s">
+        <v>2</v>
+      </c>
+      <c r="W26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" t="s">
+        <v>15</v>
+      </c>
+      <c r="K27" t="s">
+        <v>8</v>
+      </c>
+      <c r="L27" t="s">
+        <v>6</v>
+      </c>
+      <c r="M27" t="s">
+        <v>2</v>
+      </c>
+      <c r="N27" t="s">
+        <v>2</v>
+      </c>
+      <c r="O27" t="s">
+        <v>9</v>
+      </c>
+      <c r="P27" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>0</v>
+      </c>
+      <c r="R27" t="s">
+        <v>9</v>
+      </c>
+      <c r="S27" t="s">
+        <v>10</v>
+      </c>
+      <c r="T27" t="s">
+        <v>0</v>
+      </c>
+      <c r="U27" t="s">
+        <v>3</v>
+      </c>
+      <c r="V27" t="s">
+        <v>3</v>
+      </c>
+      <c r="W27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" t="s">
+        <v>3</v>
+      </c>
+      <c r="K28" t="s">
+        <v>8</v>
+      </c>
+      <c r="L28" t="s">
+        <v>6</v>
+      </c>
+      <c r="M28" t="s">
+        <v>2</v>
+      </c>
+      <c r="N28" t="s">
+        <v>2</v>
+      </c>
+      <c r="O28" t="s">
+        <v>9</v>
+      </c>
+      <c r="P28" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>0</v>
+      </c>
+      <c r="R28" t="s">
+        <v>9</v>
+      </c>
+      <c r="S28" t="s">
+        <v>10</v>
+      </c>
+      <c r="T28" t="s">
+        <v>0</v>
+      </c>
+      <c r="U28" t="s">
+        <v>7</v>
+      </c>
+      <c r="V28" t="s">
+        <v>2</v>
+      </c>
+      <c r="W28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" t="s">
+        <v>5</v>
+      </c>
+      <c r="H29" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" t="s">
+        <v>9</v>
+      </c>
+      <c r="K29" t="s">
+        <v>8</v>
+      </c>
+      <c r="L29" t="s">
+        <v>6</v>
+      </c>
+      <c r="M29" t="s">
+        <v>2</v>
+      </c>
+      <c r="N29" t="s">
+        <v>2</v>
+      </c>
+      <c r="O29" t="s">
+        <v>9</v>
+      </c>
+      <c r="P29" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>0</v>
+      </c>
+      <c r="R29" t="s">
+        <v>9</v>
+      </c>
+      <c r="S29" t="s">
+        <v>10</v>
+      </c>
+      <c r="T29" t="s">
+        <v>0</v>
+      </c>
+      <c r="U29" t="s">
+        <v>3</v>
+      </c>
+      <c r="V29" t="s">
+        <v>2</v>
+      </c>
+      <c r="W29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H30" t="s">
+        <v>6</v>
+      </c>
+      <c r="I30" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" t="s">
+        <v>7</v>
+      </c>
+      <c r="K30" t="s">
+        <v>8</v>
+      </c>
+      <c r="L30" t="s">
+        <v>8</v>
+      </c>
+      <c r="M30" t="s">
+        <v>2</v>
+      </c>
+      <c r="N30" t="s">
+        <v>2</v>
+      </c>
+      <c r="O30" t="s">
+        <v>9</v>
+      </c>
+      <c r="P30" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>0</v>
+      </c>
+      <c r="R30" t="s">
+        <v>9</v>
+      </c>
+      <c r="S30" t="s">
+        <v>10</v>
+      </c>
+      <c r="T30" t="s">
+        <v>0</v>
+      </c>
+      <c r="U30" t="s">
+        <v>3</v>
+      </c>
+      <c r="V30" t="s">
+        <v>18</v>
+      </c>
+      <c r="W30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" t="s">
+        <v>3</v>
+      </c>
+      <c r="K31" t="s">
+        <v>4</v>
+      </c>
+      <c r="L31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M31" t="s">
+        <v>2</v>
+      </c>
+      <c r="N31" t="s">
+        <v>5</v>
+      </c>
+      <c r="O31" t="s">
+        <v>9</v>
+      </c>
+      <c r="P31" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>0</v>
+      </c>
+      <c r="R31" t="s">
+        <v>9</v>
+      </c>
+      <c r="S31" t="s">
+        <v>10</v>
+      </c>
+      <c r="T31" t="s">
+        <v>8</v>
+      </c>
+      <c r="U31" t="s">
+        <v>7</v>
+      </c>
+      <c r="V31" t="s">
+        <v>13</v>
+      </c>
+      <c r="W31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" t="s">
+        <v>7</v>
+      </c>
+      <c r="K32" t="s">
+        <v>8</v>
+      </c>
+      <c r="L32" t="s">
+        <v>8</v>
+      </c>
+      <c r="M32" t="s">
+        <v>2</v>
+      </c>
+      <c r="N32" t="s">
+        <v>2</v>
+      </c>
+      <c r="O32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>0</v>
+      </c>
+      <c r="R32" t="s">
+        <v>9</v>
+      </c>
+      <c r="S32" t="s">
+        <v>10</v>
+      </c>
+      <c r="T32" t="s">
+        <v>0</v>
+      </c>
+      <c r="U32" t="s">
+        <v>3</v>
+      </c>
+      <c r="V32" t="s">
+        <v>12</v>
+      </c>
+      <c r="W32" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>